<commit_message>
snapshot, end of milestone 2
</commit_message>
<xml_diff>
--- a/_VID28 Motor/vid28, measurements.xlsx
+++ b/_VID28 Motor/vid28, measurements.xlsx
@@ -5,17 +5,18 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/allan/Desktop/ClockWall/VID28 Series Stepper Motor/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/allan/Desktop/ClockWall/ClockWall/_VID28 Motor/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="13680" yWindow="460" windowWidth="14840" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="11660" yWindow="540" windowWidth="19360" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="RLED">Sheet1!$B$75</definedName>
+    <definedName name="RLED2">Sheet1!$C$105</definedName>
     <definedName name="RPIN">Sheet1!$B$76</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="110">
   <si>
     <t>Allan Schwartz</t>
   </si>
@@ -252,12 +253,6 @@
     <t>https://github.com/adafruit/Adafruit-NeoPixel-Ring/blob/master/Adafruit%20NeoPixel%20Ring%2012.brd</t>
   </si>
   <si>
-    <t xml:space="preserve">but I can't figure out how to specify the 4 contacts, except by measuring with my calipers.   The problem is, </t>
-  </si>
-  <si>
-    <t>what should be the reference point?  How do I accurately measure?</t>
-  </si>
-  <si>
     <t>RLED</t>
   </si>
   <si>
@@ -322,6 +317,48 @@
   </si>
   <si>
     <t>radians</t>
+  </si>
+  <si>
+    <t>Install my own LEDS</t>
+  </si>
+  <si>
+    <t>Radius to center of LED</t>
+  </si>
+  <si>
+    <t>D6</t>
+  </si>
+  <si>
+    <t>D5</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>D7</t>
+  </si>
+  <si>
+    <t>D8</t>
+  </si>
+  <si>
+    <t>D9</t>
+  </si>
+  <si>
+    <t>D10</t>
+  </si>
+  <si>
+    <t>D11</t>
+  </si>
+  <si>
+    <t>D12</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>D2</t>
   </si>
 </sst>
 </file>
@@ -754,10 +791,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H105"/>
+  <dimension ref="A1:H120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="D95" sqref="D95"/>
+    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
+      <selection activeCell="C106" sqref="C106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1104,7 +1141,7 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B75">
         <f>30/2</f>
@@ -1113,7 +1150,7 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B76">
         <f>34.5/2</f>
@@ -1127,7 +1164,7 @@
     </row>
     <row r="79" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C79" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D79" s="3" t="s">
         <v>29</v>
@@ -1147,16 +1184,16 @@
         <v>2</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D80" s="4" t="s">
         <v>5</v>
       </c>
       <c r="E80" s="6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F80" s="4" t="s">
         <v>6</v>
@@ -1168,9 +1205,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B82">
         <v>0</v>
@@ -1187,10 +1224,14 @@
         <f>RLED*SIN(C82)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G82">
+        <f>D82+17.5</f>
+        <v>32.5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B83">
         <f>B82+30</f>
@@ -1209,9 +1250,9 @@
         <v>7.4999999999999991</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B84">
         <f t="shared" ref="B84:B96" si="1">B83+30</f>
@@ -1230,9 +1271,9 @@
         <v>12.990381056766578</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B85">
         <f t="shared" si="1"/>
@@ -1251,9 +1292,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="86" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A86" s="7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B86" s="7">
         <f>B85+15</f>
@@ -1272,9 +1313,9 @@
         <v>16.662220503486427</v>
       </c>
     </row>
-    <row r="87" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A87" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B87" s="5">
         <f>B85+30</f>
@@ -1293,9 +1334,9 @@
         <v>12.99038105676658</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B88">
         <f t="shared" si="1"/>
@@ -1314,9 +1355,9 @@
         <v>7.4999999999999991</v>
       </c>
     </row>
-    <row r="89" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A89" s="7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B89" s="7">
         <f>B88+15</f>
@@ -1335,9 +1376,9 @@
         <v>4.4646285280184879</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B90">
         <f>B88+30</f>
@@ -1356,9 +1397,9 @@
         <v>1.83772268236293E-15</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B91">
         <f t="shared" si="1"/>
@@ -1377,9 +1418,9 @@
         <v>-7.5000000000000018</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B92">
         <f t="shared" si="1"/>
@@ -1398,9 +1439,9 @@
         <v>-12.990381056766577</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B93">
         <f t="shared" si="1"/>
@@ -1419,9 +1460,9 @@
         <v>-15</v>
       </c>
     </row>
-    <row r="94" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A94" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B94" s="7">
         <f>B93+15</f>
@@ -1440,9 +1481,9 @@
         <v>-16.662220503486431</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B95">
         <f>B93+30</f>
@@ -1461,9 +1502,9 @@
         <v>-12.990381056766578</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B96">
         <f t="shared" si="1"/>
@@ -1482,9 +1523,9 @@
         <v>-7.5000000000000071</v>
       </c>
     </row>
-    <row r="97" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A97" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B97" s="7">
         <f>B96+15</f>
@@ -1503,28 +1544,328 @@
         <v>-4.4646285280184816</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>75</v>
+        <v>97</v>
+      </c>
+      <c r="C105">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C106" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D106" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F106" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G106" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H106" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A107" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B107" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C107" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D107" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E107" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F107" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G107" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H107" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>101</v>
+      </c>
+      <c r="B109">
+        <v>0</v>
+      </c>
+      <c r="C109">
+        <f>RADIANS(B109)</f>
+        <v>0</v>
+      </c>
+      <c r="D109">
+        <f>RLED2*COS(C109)</f>
+        <v>21</v>
+      </c>
+      <c r="E109">
+        <f>RLED2*SIN(C109)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>100</v>
+      </c>
+      <c r="B110">
+        <f>B109+30</f>
+        <v>30</v>
+      </c>
+      <c r="C110">
+        <f t="shared" ref="C110:C112" si="5">RADIANS(B110)</f>
+        <v>0.52359877559829882</v>
+      </c>
+      <c r="D110">
+        <f>RLED2*COS(C110)</f>
+        <v>18.186533479473212</v>
+      </c>
+      <c r="E110">
+        <f>RLED2*SIN(C110)</f>
+        <v>10.499999999999998</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>99</v>
+      </c>
+      <c r="B111">
+        <f t="shared" ref="B111:B120" si="6">B110+30</f>
+        <v>60</v>
+      </c>
+      <c r="C111">
+        <f t="shared" si="5"/>
+        <v>1.0471975511965976</v>
+      </c>
+      <c r="D111">
+        <f>RLED2*COS(C111)</f>
+        <v>10.500000000000002</v>
+      </c>
+      <c r="E111">
+        <f>RLED2*SIN(C111)</f>
+        <v>18.186533479473212</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>98</v>
+      </c>
+      <c r="B112">
+        <f t="shared" si="6"/>
+        <v>90</v>
+      </c>
+      <c r="C112">
+        <f t="shared" si="5"/>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="D112">
+        <f>RLED2*COS(C112)</f>
+        <v>1.286405877654051E-15</v>
+      </c>
+      <c r="E112">
+        <f>RLED2*SIN(C112)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A113" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B113" s="5">
+        <f>B112+30</f>
+        <v>120</v>
+      </c>
+      <c r="C113">
+        <f t="shared" ref="C113:C114" si="7">RADIANS(B113)</f>
+        <v>2.0943951023931953</v>
+      </c>
+      <c r="D113">
+        <f>RLED2*COS(C113)</f>
+        <v>-10.499999999999995</v>
+      </c>
+      <c r="E113">
+        <f>RLED2*SIN(C113)</f>
+        <v>18.186533479473212</v>
+      </c>
+      <c r="G113"/>
+      <c r="H113"/>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>103</v>
+      </c>
+      <c r="B114">
+        <f t="shared" si="6"/>
+        <v>150</v>
+      </c>
+      <c r="C114">
+        <f t="shared" si="7"/>
+        <v>2.6179938779914944</v>
+      </c>
+      <c r="D114">
+        <f>RLED2*COS(C114)</f>
+        <v>-18.186533479473212</v>
+      </c>
+      <c r="E114">
+        <f>RLED2*SIN(C114)</f>
+        <v>10.499999999999998</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>104</v>
+      </c>
+      <c r="B115">
+        <f>B114+30</f>
+        <v>180</v>
+      </c>
+      <c r="C115">
+        <f t="shared" ref="C115:C118" si="8">RADIANS(B115)</f>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="D115">
+        <f>RLED2*COS(C115)</f>
+        <v>-21</v>
+      </c>
+      <c r="E115">
+        <f>RLED2*SIN(C115)</f>
+        <v>2.572811755308102E-15</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>105</v>
+      </c>
+      <c r="B116">
+        <f t="shared" si="6"/>
+        <v>210</v>
+      </c>
+      <c r="C116">
+        <f t="shared" si="8"/>
+        <v>3.6651914291880923</v>
+      </c>
+      <c r="D116">
+        <f>RLED2*COS(C116)</f>
+        <v>-18.186533479473212</v>
+      </c>
+      <c r="E116">
+        <f>RLED2*SIN(C116)</f>
+        <v>-10.500000000000002</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>106</v>
+      </c>
+      <c r="B117">
+        <f t="shared" si="6"/>
+        <v>240</v>
+      </c>
+      <c r="C117">
+        <f t="shared" si="8"/>
+        <v>4.1887902047863905</v>
+      </c>
+      <c r="D117">
+        <f>RLED2*COS(C117)</f>
+        <v>-10.500000000000009</v>
+      </c>
+      <c r="E117">
+        <f>RLED2*SIN(C117)</f>
+        <v>-18.186533479473205</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>107</v>
+      </c>
+      <c r="B118">
+        <f t="shared" si="6"/>
+        <v>270</v>
+      </c>
+      <c r="C118">
+        <f t="shared" si="8"/>
+        <v>4.7123889803846897</v>
+      </c>
+      <c r="D118">
+        <f>RLED2*COS(C118)</f>
+        <v>-3.859217632962153E-15</v>
+      </c>
+      <c r="E118">
+        <f>RLED2*SIN(C118)</f>
+        <v>-21</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>108</v>
+      </c>
+      <c r="B119">
+        <f>B118+30</f>
+        <v>300</v>
+      </c>
+      <c r="C119">
+        <f t="shared" ref="C119:C120" si="9">RADIANS(B119)</f>
+        <v>5.2359877559829888</v>
+      </c>
+      <c r="D119">
+        <f>RLED2*COS(C119)</f>
+        <v>10.500000000000002</v>
+      </c>
+      <c r="E119">
+        <f>RLED2*SIN(C119)</f>
+        <v>-18.186533479473212</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>109</v>
+      </c>
+      <c r="B120">
+        <f t="shared" si="6"/>
+        <v>330</v>
+      </c>
+      <c r="C120">
+        <f t="shared" si="9"/>
+        <v>5.7595865315812871</v>
+      </c>
+      <c r="D120">
+        <f>RLED2*COS(C120)</f>
+        <v>18.186533479473205</v>
+      </c>
+      <c r="E120">
+        <f>RLED2*SIN(C120)</f>
+        <v>-10.500000000000009</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <ignoredErrors>
     <ignoredError sqref="D86 D89 D94" formula="1"/>
   </ignoredErrors>

</xml_diff>